<commit_message>
añadi el control por aumento de latitud
</commit_message>
<xml_diff>
--- a/Logs/logreg1-9-3-18.xlsx
+++ b/Logs/logreg1-9-3-18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WVALDOGRAELL\Documents\GitHub\RETO_I2C\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36E95A0-19CF-4471-902E-8D521A747B2C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFA709C-48E7-4B70-997A-9ED3E040389C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2293,19 +2293,19 @@
     <t>9.0231772, -79.5314817, 3, Region 1</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Region 1</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Distancia</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -7026,7 +7026,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr u="none"/>
       </a:pPr>
       <a:endParaRPr lang="es-PA"/>
     </a:p>
@@ -9267,16 +9267,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9304,15 +9304,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>347662</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>347662</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9340,15 +9340,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>423862</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>423862</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9375,16 +9375,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9429,10 +9429,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="logreg1" displayName="logreg1" ref="A1:D491" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D491" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Latitud" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Longitud" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Distancia" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Region" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9737,8 +9737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9750,16 +9750,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -9773,7 +9773,7 @@
         <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9787,7 +9787,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -9801,7 +9801,7 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -9815,7 +9815,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -9829,7 +9829,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -9843,7 +9843,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -9857,7 +9857,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -9871,7 +9871,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9885,7 +9885,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9899,7 +9899,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -9913,7 +9913,7 @@
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -9927,7 +9927,7 @@
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -9941,7 +9941,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -9955,7 +9955,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -9969,7 +9969,7 @@
         <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -9983,7 +9983,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -9997,7 +9997,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10011,7 +10011,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -10025,7 +10025,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -10039,7 +10039,7 @@
         <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -10053,7 +10053,7 @@
         <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -10067,7 +10067,7 @@
         <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -10081,7 +10081,7 @@
         <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -10095,7 +10095,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -10109,7 +10109,7 @@
         <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -10123,7 +10123,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -10137,7 +10137,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -10151,7 +10151,7 @@
         <v>27</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -10165,7 +10165,7 @@
         <v>27</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -10179,7 +10179,7 @@
         <v>26</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -10193,7 +10193,7 @@
         <v>26</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -10207,7 +10207,7 @@
         <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -10221,7 +10221,7 @@
         <v>26</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -10235,7 +10235,7 @@
         <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -10249,7 +10249,7 @@
         <v>25</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -10263,7 +10263,7 @@
         <v>25</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -10277,7 +10277,7 @@
         <v>25</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -10291,7 +10291,7 @@
         <v>25</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -10305,7 +10305,7 @@
         <v>25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -10319,7 +10319,7 @@
         <v>25</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -10333,7 +10333,7 @@
         <v>25</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -10347,7 +10347,7 @@
         <v>25</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -10361,7 +10361,7 @@
         <v>25</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>24</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -10389,7 +10389,7 @@
         <v>24</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -10403,7 +10403,7 @@
         <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -10417,7 +10417,7 @@
         <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -10431,7 +10431,7 @@
         <v>23</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -10445,7 +10445,7 @@
         <v>23</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -10459,7 +10459,7 @@
         <v>23</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -10473,7 +10473,7 @@
         <v>23</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>22</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -10501,7 +10501,7 @@
         <v>23</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -10515,7 +10515,7 @@
         <v>22</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -10529,7 +10529,7 @@
         <v>22</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -10543,7 +10543,7 @@
         <v>21</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -10557,7 +10557,7 @@
         <v>21</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -10571,7 +10571,7 @@
         <v>21</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -10585,7 +10585,7 @@
         <v>20</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -10599,7 +10599,7 @@
         <v>20</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -10613,7 +10613,7 @@
         <v>20</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -10627,7 +10627,7 @@
         <v>20</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -10641,7 +10641,7 @@
         <v>19</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -10655,7 +10655,7 @@
         <v>19</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -10669,7 +10669,7 @@
         <v>19</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -10683,7 +10683,7 @@
         <v>19</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -10697,7 +10697,7 @@
         <v>19</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -10711,7 +10711,7 @@
         <v>19</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -10725,7 +10725,7 @@
         <v>19</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -10739,7 +10739,7 @@
         <v>19</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -10753,7 +10753,7 @@
         <v>18</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>18</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -10781,7 +10781,7 @@
         <v>18</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -10795,7 +10795,7 @@
         <v>18</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -10809,7 +10809,7 @@
         <v>18</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>18</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -10837,7 +10837,7 @@
         <v>18</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -10851,7 +10851,7 @@
         <v>17</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -10865,7 +10865,7 @@
         <v>17</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>17</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -10893,7 +10893,7 @@
         <v>17</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -10907,7 +10907,7 @@
         <v>17</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -10921,7 +10921,7 @@
         <v>17</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>17</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -10949,7 +10949,7 @@
         <v>17</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -10963,7 +10963,7 @@
         <v>16</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -10977,7 +10977,7 @@
         <v>16</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>16</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -11005,7 +11005,7 @@
         <v>16</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -11019,7 +11019,7 @@
         <v>16</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -11033,7 +11033,7 @@
         <v>16</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>16</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -11061,7 +11061,7 @@
         <v>16</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -11075,7 +11075,7 @@
         <v>15</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -11089,7 +11089,7 @@
         <v>15</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>15</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -11117,7 +11117,7 @@
         <v>15</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -11131,7 +11131,7 @@
         <v>15</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -11145,7 +11145,7 @@
         <v>14</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>14</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -11173,7 +11173,7 @@
         <v>14</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -11187,7 +11187,7 @@
         <v>14</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -11201,7 +11201,7 @@
         <v>14</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>14</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -11229,7 +11229,7 @@
         <v>14</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -11243,7 +11243,7 @@
         <v>14</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -11257,7 +11257,7 @@
         <v>13</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>13</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -11285,7 +11285,7 @@
         <v>13</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -11299,7 +11299,7 @@
         <v>12</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -11313,7 +11313,7 @@
         <v>12</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -11327,7 +11327,7 @@
         <v>12</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -11341,7 +11341,7 @@
         <v>11</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -11355,7 +11355,7 @@
         <v>11</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -11369,7 +11369,7 @@
         <v>11</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>11</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -11397,7 +11397,7 @@
         <v>11</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -11411,7 +11411,7 @@
         <v>10</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -11425,7 +11425,7 @@
         <v>10</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -11439,7 +11439,7 @@
         <v>10</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -11453,7 +11453,7 @@
         <v>10</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -11467,7 +11467,7 @@
         <v>10</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -11481,7 +11481,7 @@
         <v>10</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>9</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -11509,7 +11509,7 @@
         <v>9</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -11523,7 +11523,7 @@
         <v>9</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -11537,7 +11537,7 @@
         <v>9</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>9</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -11565,7 +11565,7 @@
         <v>9</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -11579,7 +11579,7 @@
         <v>9</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -11593,7 +11593,7 @@
         <v>9</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -11607,7 +11607,7 @@
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -11621,7 +11621,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -11635,7 +11635,7 @@
         <v>8</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -11649,7 +11649,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -11663,7 +11663,7 @@
         <v>7</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -11677,7 +11677,7 @@
         <v>7</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -11691,7 +11691,7 @@
         <v>7</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -11705,7 +11705,7 @@
         <v>7</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>7</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -11733,7 +11733,7 @@
         <v>7</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -11747,7 +11747,7 @@
         <v>7</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -11761,7 +11761,7 @@
         <v>7</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -11775,7 +11775,7 @@
         <v>7</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -11789,7 +11789,7 @@
         <v>7</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -11803,7 +11803,7 @@
         <v>7</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -11817,7 +11817,7 @@
         <v>7</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>6</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -11845,7 +11845,7 @@
         <v>6</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -11859,7 +11859,7 @@
         <v>6</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -11873,7 +11873,7 @@
         <v>5</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -11901,7 +11901,7 @@
         <v>5</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -11915,7 +11915,7 @@
         <v>5</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -11929,7 +11929,7 @@
         <v>5</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>5</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -11957,7 +11957,7 @@
         <v>5</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -11971,7 +11971,7 @@
         <v>5</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -11985,7 +11985,7 @@
         <v>5</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>5</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -12013,7 +12013,7 @@
         <v>4</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -12027,7 +12027,7 @@
         <v>5</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -12041,7 +12041,7 @@
         <v>4</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>4</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -12069,7 +12069,7 @@
         <v>4</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -12083,7 +12083,7 @@
         <v>4</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -12097,7 +12097,7 @@
         <v>4</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -12111,7 +12111,7 @@
         <v>3</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -12125,7 +12125,7 @@
         <v>3</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -12139,7 +12139,7 @@
         <v>3</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -12153,7 +12153,7 @@
         <v>3</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -12181,7 +12181,7 @@
         <v>3</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -12195,7 +12195,7 @@
         <v>3</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -12209,7 +12209,7 @@
         <v>3</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -12223,7 +12223,7 @@
         <v>3</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -12237,7 +12237,7 @@
         <v>3</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -12251,7 +12251,7 @@
         <v>3</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -12265,7 +12265,7 @@
         <v>3</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>3</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -12293,7 +12293,7 @@
         <v>3</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -12307,7 +12307,7 @@
         <v>3</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -12321,7 +12321,7 @@
         <v>3</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>3</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -12349,7 +12349,7 @@
         <v>3</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -12363,7 +12363,7 @@
         <v>4</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -12377,7 +12377,7 @@
         <v>4</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>4</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -12405,7 +12405,7 @@
         <v>4</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -12419,7 +12419,7 @@
         <v>4</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -12433,7 +12433,7 @@
         <v>3</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>3</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -12461,7 +12461,7 @@
         <v>3</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -12475,7 +12475,7 @@
         <v>2</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -12489,7 +12489,7 @@
         <v>10</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>10</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -12517,7 +12517,7 @@
         <v>10</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -12531,7 +12531,7 @@
         <v>10</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -12545,7 +12545,7 @@
         <v>9</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>9</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -12573,7 +12573,7 @@
         <v>9</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -12587,7 +12587,7 @@
         <v>9</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -12601,7 +12601,7 @@
         <v>9</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>9</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -12629,7 +12629,7 @@
         <v>9</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -12643,7 +12643,7 @@
         <v>9</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -12657,7 +12657,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -12671,7 +12671,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -12685,7 +12685,7 @@
         <v>8</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -12699,7 +12699,7 @@
         <v>8</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -12713,7 +12713,7 @@
         <v>8</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -12741,7 +12741,7 @@
         <v>8</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -12755,7 +12755,7 @@
         <v>7</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -12769,7 +12769,7 @@
         <v>7</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -12783,7 +12783,7 @@
         <v>7</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -12797,7 +12797,7 @@
         <v>7</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -12811,7 +12811,7 @@
         <v>7</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -12825,7 +12825,7 @@
         <v>7</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -12839,7 +12839,7 @@
         <v>6</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -12853,7 +12853,7 @@
         <v>6</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -12867,7 +12867,7 @@
         <v>6</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -12881,7 +12881,7 @@
         <v>6</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -12895,7 +12895,7 @@
         <v>6</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -12909,7 +12909,7 @@
         <v>6</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -12923,7 +12923,7 @@
         <v>5</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -12937,7 +12937,7 @@
         <v>5</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>5</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -12965,7 +12965,7 @@
         <v>5</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -12979,7 +12979,7 @@
         <v>4</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -12993,7 +12993,7 @@
         <v>4</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>4</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -13021,7 +13021,7 @@
         <v>4</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -13035,7 +13035,7 @@
         <v>4</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -13049,7 +13049,7 @@
         <v>4</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -13063,7 +13063,7 @@
         <v>4</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -13077,7 +13077,7 @@
         <v>4</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -13091,7 +13091,7 @@
         <v>4</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -13105,7 +13105,7 @@
         <v>3</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -13119,7 +13119,7 @@
         <v>3</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -13133,7 +13133,7 @@
         <v>3</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -13147,7 +13147,7 @@
         <v>3</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -13161,7 +13161,7 @@
         <v>3</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -13175,7 +13175,7 @@
         <v>4</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -13189,7 +13189,7 @@
         <v>3</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -13203,7 +13203,7 @@
         <v>3</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -13217,7 +13217,7 @@
         <v>3</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -13231,7 +13231,7 @@
         <v>4</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -13245,7 +13245,7 @@
         <v>4</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -13259,7 +13259,7 @@
         <v>4</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -13273,7 +13273,7 @@
         <v>4</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -13287,7 +13287,7 @@
         <v>30</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -13301,7 +13301,7 @@
         <v>30</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -13315,7 +13315,7 @@
         <v>30</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -13329,7 +13329,7 @@
         <v>30</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -13343,7 +13343,7 @@
         <v>31</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -13357,7 +13357,7 @@
         <v>31</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -13371,7 +13371,7 @@
         <v>32</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -13385,7 +13385,7 @@
         <v>32</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -13399,7 +13399,7 @@
         <v>32</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -13413,7 +13413,7 @@
         <v>32</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -13427,7 +13427,7 @@
         <v>32</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
@@ -13441,7 +13441,7 @@
         <v>31</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
@@ -13455,7 +13455,7 @@
         <v>31</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -13469,7 +13469,7 @@
         <v>31</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
@@ -13483,7 +13483,7 @@
         <v>31</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -13497,7 +13497,7 @@
         <v>30</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -13511,7 +13511,7 @@
         <v>30</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -13525,7 +13525,7 @@
         <v>30</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -13539,7 +13539,7 @@
         <v>30</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -13553,7 +13553,7 @@
         <v>30</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -13567,7 +13567,7 @@
         <v>29</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -13581,7 +13581,7 @@
         <v>29</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -13595,7 +13595,7 @@
         <v>29</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -13609,7 +13609,7 @@
         <v>29</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -13623,7 +13623,7 @@
         <v>28</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
@@ -13637,7 +13637,7 @@
         <v>28</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -13651,7 +13651,7 @@
         <v>28</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -13665,7 +13665,7 @@
         <v>28</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -13679,7 +13679,7 @@
         <v>28</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -13693,7 +13693,7 @@
         <v>27</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -13707,7 +13707,7 @@
         <v>27</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -13721,7 +13721,7 @@
         <v>27</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -13735,7 +13735,7 @@
         <v>27</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -13749,7 +13749,7 @@
         <v>27</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -13763,7 +13763,7 @@
         <v>27</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
@@ -13777,7 +13777,7 @@
         <v>26</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -13791,7 +13791,7 @@
         <v>26</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -13805,7 +13805,7 @@
         <v>26</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -13819,7 +13819,7 @@
         <v>26</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -13833,7 +13833,7 @@
         <v>25</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -13847,7 +13847,7 @@
         <v>25</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
@@ -13861,7 +13861,7 @@
         <v>25</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -13875,7 +13875,7 @@
         <v>25</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
@@ -13889,7 +13889,7 @@
         <v>24</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
@@ -13903,7 +13903,7 @@
         <v>24</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -13917,7 +13917,7 @@
         <v>24</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -13931,7 +13931,7 @@
         <v>24</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -13945,7 +13945,7 @@
         <v>24</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -13959,7 +13959,7 @@
         <v>23</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
@@ -13973,7 +13973,7 @@
         <v>23</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -13987,7 +13987,7 @@
         <v>23</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
@@ -14001,7 +14001,7 @@
         <v>23</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
@@ -14015,7 +14015,7 @@
         <v>23</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -14029,7 +14029,7 @@
         <v>23</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -14043,7 +14043,7 @@
         <v>22</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -14057,7 +14057,7 @@
         <v>22</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -14071,7 +14071,7 @@
         <v>22</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -14085,7 +14085,7 @@
         <v>22</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -14099,7 +14099,7 @@
         <v>22</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -14113,7 +14113,7 @@
         <v>21</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -14127,7 +14127,7 @@
         <v>21</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
@@ -14141,7 +14141,7 @@
         <v>21</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -14155,7 +14155,7 @@
         <v>21</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
@@ -14169,7 +14169,7 @@
         <v>21</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -14183,7 +14183,7 @@
         <v>21</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -14197,7 +14197,7 @@
         <v>20</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -14211,7 +14211,7 @@
         <v>20</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -14225,7 +14225,7 @@
         <v>20</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -14239,7 +14239,7 @@
         <v>20</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
@@ -14253,7 +14253,7 @@
         <v>20</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
@@ -14267,7 +14267,7 @@
         <v>20</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -14281,7 +14281,7 @@
         <v>20</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -14295,7 +14295,7 @@
         <v>20</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -14309,7 +14309,7 @@
         <v>20</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -14323,7 +14323,7 @@
         <v>19</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -14337,7 +14337,7 @@
         <v>19</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -14351,7 +14351,7 @@
         <v>19</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -14365,7 +14365,7 @@
         <v>19</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -14379,7 +14379,7 @@
         <v>19</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
@@ -14393,7 +14393,7 @@
         <v>19</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -14407,7 +14407,7 @@
         <v>19</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -14421,7 +14421,7 @@
         <v>19</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -14435,7 +14435,7 @@
         <v>19</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -14449,7 +14449,7 @@
         <v>19</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -14463,7 +14463,7 @@
         <v>18</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -14477,7 +14477,7 @@
         <v>18</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -14491,7 +14491,7 @@
         <v>18</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -14505,7 +14505,7 @@
         <v>18</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -14519,7 +14519,7 @@
         <v>18</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -14533,7 +14533,7 @@
         <v>17</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -14547,7 +14547,7 @@
         <v>17</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -14561,7 +14561,7 @@
         <v>17</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -14575,7 +14575,7 @@
         <v>17</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -14589,7 +14589,7 @@
         <v>17</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
@@ -14603,7 +14603,7 @@
         <v>17</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
@@ -14617,7 +14617,7 @@
         <v>17</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -14631,7 +14631,7 @@
         <v>16</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -14645,7 +14645,7 @@
         <v>16</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -14659,7 +14659,7 @@
         <v>16</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -14673,7 +14673,7 @@
         <v>16</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -14687,7 +14687,7 @@
         <v>16</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -14701,7 +14701,7 @@
         <v>15</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -14715,7 +14715,7 @@
         <v>15</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -14729,7 +14729,7 @@
         <v>15</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -14743,7 +14743,7 @@
         <v>15</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -14757,7 +14757,7 @@
         <v>15</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -14771,7 +14771,7 @@
         <v>15</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -14785,7 +14785,7 @@
         <v>15</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -14799,7 +14799,7 @@
         <v>14</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -14813,7 +14813,7 @@
         <v>14</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -14827,7 +14827,7 @@
         <v>14</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -14841,7 +14841,7 @@
         <v>14</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -14855,7 +14855,7 @@
         <v>14</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -14869,7 +14869,7 @@
         <v>14</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -14883,7 +14883,7 @@
         <v>13</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -14897,7 +14897,7 @@
         <v>13</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -14911,7 +14911,7 @@
         <v>13</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -14925,7 +14925,7 @@
         <v>13</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
@@ -14939,7 +14939,7 @@
         <v>12</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -14953,7 +14953,7 @@
         <v>12</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -14967,7 +14967,7 @@
         <v>12</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -14981,7 +14981,7 @@
         <v>12</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -14995,7 +14995,7 @@
         <v>12</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -15009,7 +15009,7 @@
         <v>12</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -15023,7 +15023,7 @@
         <v>11</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -15037,7 +15037,7 @@
         <v>11</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -15051,7 +15051,7 @@
         <v>11</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -15065,7 +15065,7 @@
         <v>11</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -15079,7 +15079,7 @@
         <v>11</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -15093,7 +15093,7 @@
         <v>11</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -15107,7 +15107,7 @@
         <v>11</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -15121,7 +15121,7 @@
         <v>11</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
@@ -15135,7 +15135,7 @@
         <v>10</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
@@ -15149,7 +15149,7 @@
         <v>10</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
@@ -15163,7 +15163,7 @@
         <v>10</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
@@ -15177,7 +15177,7 @@
         <v>10</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
@@ -15191,7 +15191,7 @@
         <v>10</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
@@ -15205,7 +15205,7 @@
         <v>10</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -15216,7 +15216,7 @@
         <v>7</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
@@ -15230,7 +15230,7 @@
         <v>7</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
@@ -15244,7 +15244,7 @@
         <v>7</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
@@ -15258,7 +15258,7 @@
         <v>7</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
@@ -15272,7 +15272,7 @@
         <v>7</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
@@ -15286,7 +15286,7 @@
         <v>7</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
@@ -15300,7 +15300,7 @@
         <v>7</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
@@ -15314,7 +15314,7 @@
         <v>7</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
@@ -15328,7 +15328,7 @@
         <v>7</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
@@ -15342,7 +15342,7 @@
         <v>6</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
@@ -15356,7 +15356,7 @@
         <v>6</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -15370,7 +15370,7 @@
         <v>6</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
@@ -15384,7 +15384,7 @@
         <v>6</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
@@ -15398,7 +15398,7 @@
         <v>6</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
@@ -15412,7 +15412,7 @@
         <v>6</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
@@ -15426,7 +15426,7 @@
         <v>5</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -15440,7 +15440,7 @@
         <v>5</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
@@ -15454,7 +15454,7 @@
         <v>5</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
@@ -15468,7 +15468,7 @@
         <v>4</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
@@ -15482,7 +15482,7 @@
         <v>4</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
@@ -15496,7 +15496,7 @@
         <v>4</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
@@ -15510,7 +15510,7 @@
         <v>4</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
@@ -15524,7 +15524,7 @@
         <v>4</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
@@ -15538,7 +15538,7 @@
         <v>4</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
@@ -15552,7 +15552,7 @@
         <v>3</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
@@ -15566,7 +15566,7 @@
         <v>3</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
@@ -15580,7 +15580,7 @@
         <v>3</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
@@ -15594,7 +15594,7 @@
         <v>3</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
@@ -15608,7 +15608,7 @@
         <v>3</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
@@ -15622,7 +15622,7 @@
         <v>3</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
@@ -15636,7 +15636,7 @@
         <v>3</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
@@ -15650,7 +15650,7 @@
         <v>3</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
@@ -15664,7 +15664,7 @@
         <v>3</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
@@ -15678,7 +15678,7 @@
         <v>3</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
@@ -15692,7 +15692,7 @@
         <v>3</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
@@ -15706,7 +15706,7 @@
         <v>3</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
@@ -15720,7 +15720,7 @@
         <v>3</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
@@ -15734,7 +15734,7 @@
         <v>3</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
@@ -15748,7 +15748,7 @@
         <v>3</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
@@ -15762,7 +15762,7 @@
         <v>3</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
@@ -15776,7 +15776,7 @@
         <v>3</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
@@ -15790,7 +15790,7 @@
         <v>4</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
@@ -15804,7 +15804,7 @@
         <v>4</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
@@ -15818,7 +15818,7 @@
         <v>4</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
@@ -15832,7 +15832,7 @@
         <v>4</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
@@ -15846,7 +15846,7 @@
         <v>4</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
@@ -15860,7 +15860,7 @@
         <v>4</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
@@ -15874,7 +15874,7 @@
         <v>14</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
@@ -15888,7 +15888,7 @@
         <v>14</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
@@ -15902,7 +15902,7 @@
         <v>14</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
@@ -15916,7 +15916,7 @@
         <v>14</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
@@ -15930,7 +15930,7 @@
         <v>14</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
@@ -15944,7 +15944,7 @@
         <v>14</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
@@ -15958,7 +15958,7 @@
         <v>14</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -15972,7 +15972,7 @@
         <v>13</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -15986,7 +15986,7 @@
         <v>13</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -16000,7 +16000,7 @@
         <v>13</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -16014,7 +16014,7 @@
         <v>13</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
@@ -16028,7 +16028,7 @@
         <v>12</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.25">
@@ -16042,7 +16042,7 @@
         <v>12</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.25">
@@ -16056,7 +16056,7 @@
         <v>12</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.25">
@@ -16070,7 +16070,7 @@
         <v>12</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.25">
@@ -16084,7 +16084,7 @@
         <v>11</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.25">
@@ -16098,7 +16098,7 @@
         <v>11</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.25">
@@ -16112,7 +16112,7 @@
         <v>11</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.25">
@@ -16126,7 +16126,7 @@
         <v>11</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.25">
@@ -16140,7 +16140,7 @@
         <v>11</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.25">
@@ -16154,7 +16154,7 @@
         <v>11</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
@@ -16168,7 +16168,7 @@
         <v>10</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.25">
@@ -16182,7 +16182,7 @@
         <v>10</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.25">
@@ -16196,7 +16196,7 @@
         <v>10</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
@@ -16210,7 +16210,7 @@
         <v>10</v>
       </c>
       <c r="D462" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.25">
@@ -16224,7 +16224,7 @@
         <v>10</v>
       </c>
       <c r="D463" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.25">
@@ -16238,7 +16238,7 @@
         <v>10</v>
       </c>
       <c r="D464" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.25">
@@ -16252,7 +16252,7 @@
         <v>10</v>
       </c>
       <c r="D465" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.25">
@@ -16266,7 +16266,7 @@
         <v>9</v>
       </c>
       <c r="D466" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.25">
@@ -16280,7 +16280,7 @@
         <v>9</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.25">
@@ -16294,7 +16294,7 @@
         <v>9</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
@@ -16308,7 +16308,7 @@
         <v>9</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
@@ -16322,7 +16322,7 @@
         <v>9</v>
       </c>
       <c r="D470" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
@@ -16336,7 +16336,7 @@
         <v>9</v>
       </c>
       <c r="D471" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
@@ -16350,7 +16350,7 @@
         <v>9</v>
       </c>
       <c r="D472" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
@@ -16364,7 +16364,7 @@
         <v>8</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.25">
@@ -16378,7 +16378,7 @@
         <v>8</v>
       </c>
       <c r="D474" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.25">
@@ -16392,7 +16392,7 @@
         <v>8</v>
       </c>
       <c r="D475" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
@@ -16406,7 +16406,7 @@
         <v>8</v>
       </c>
       <c r="D476" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
@@ -16420,7 +16420,7 @@
         <v>7</v>
       </c>
       <c r="D477" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
@@ -16434,7 +16434,7 @@
         <v>7</v>
       </c>
       <c r="D478" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
@@ -16448,7 +16448,7 @@
         <v>7</v>
       </c>
       <c r="D479" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
@@ -16462,7 +16462,7 @@
         <v>7</v>
       </c>
       <c r="D480" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
@@ -16476,7 +16476,7 @@
         <v>7</v>
       </c>
       <c r="D481" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.25">
@@ -16490,7 +16490,7 @@
         <v>7</v>
       </c>
       <c r="D482" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.25">
@@ -16504,7 +16504,7 @@
         <v>7</v>
       </c>
       <c r="D483" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.25">
@@ -16518,7 +16518,7 @@
         <v>7</v>
       </c>
       <c r="D484" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.25">
@@ -16532,7 +16532,7 @@
         <v>7</v>
       </c>
       <c r="D485" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.25">
@@ -16546,7 +16546,7 @@
         <v>7</v>
       </c>
       <c r="D486" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
@@ -16560,7 +16560,7 @@
         <v>7</v>
       </c>
       <c r="D487" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
@@ -16574,7 +16574,7 @@
         <v>7</v>
       </c>
       <c r="D488" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
@@ -16588,7 +16588,7 @@
         <v>7</v>
       </c>
       <c r="D489" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
@@ -16602,7 +16602,7 @@
         <v>7</v>
       </c>
       <c r="D490" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
@@ -16616,7 +16616,7 @@
         <v>7</v>
       </c>
       <c r="D491" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>